<commit_message>
Updated with local notes to feedrates translation
</commit_message>
<xml_diff>
--- a/Songs/Gerudo Valley to G-Code.xlsx
+++ b/Songs/Gerudo Valley to G-Code.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conta\Documents\Instructables and Projects\Ender 3 Music\Musical Marlin\Songs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C34420-9985-4DEB-B65E-F14B300BA5BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1764E64-7954-46A9-AAE9-722709F3CF32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="G-Code Generator" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes to Feedrate" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -72,8 +70,80 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={6020CAEE-D306-4F1F-BB7F-A6CB184BC50D}</author>
+    <author>tc={2E6EC54C-154F-40FF-9749-75F374B15888}</author>
+    <author>tc={1528385D-5D7B-4677-AEC9-9C49986BDF3B}</author>
+    <author>tc={9F3A1DCB-0146-47AA-B870-7E7AB149BD73}</author>
+    <author>tc={BE0622C6-345E-43CD-B3D2-D7804500A6B7}</author>
+    <author>tc={84CA6D1B-466B-4B66-BFE4-2488886A4766}</author>
+    <author>tc={AA34F346-5608-41B5-BA45-AD2A51502823}</author>
+  </authors>
+  <commentList>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{6020CAEE-D306-4F1F-BB7F-A6CB184BC50D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    X-Axis maximum feedrate = 500 mm/min</t>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="1" shapeId="0" xr:uid="{2E6EC54C-154F-40FF-9749-75F374B15888}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Feedrate = (Frequency * 60) / Steps per mm</t>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="2" shapeId="0" xr:uid="{1528385D-5D7B-4677-AEC9-9C49986BDF3B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tenor C</t>
+      </text>
+    </comment>
+    <comment ref="A32" authorId="3" shapeId="0" xr:uid="{9F3A1DCB-0146-47AA-B870-7E7AB149BD73}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Middle C</t>
+      </text>
+    </comment>
+    <comment ref="A56" authorId="4" shapeId="0" xr:uid="{BE0622C6-345E-43CD-B3D2-D7804500A6B7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Deep C</t>
+      </text>
+    </comment>
+    <comment ref="A58" authorId="5" shapeId="0" xr:uid="{84CA6D1B-466B-4B66-BFE4-2488886A4766}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Rest</t>
+      </text>
+    </comment>
+    <comment ref="B58" authorId="6" shapeId="0" xr:uid="{AA34F346-5608-41B5-BA45-AD2A51502823}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This frequency is too low for human hearing to detect.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="66">
   <si>
     <t>Song of Storms to G-Code</t>
   </si>
@@ -151,12 +221,173 @@
   <si>
     <t>A♭4</t>
   </si>
+  <si>
+    <t>Notes to Feedrate</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Convert musical notes, defined as frequencies (Hz), into feedrates (mm/min) given axis steps per millimeter. Driving a stepper motor at the calculated feedrate will cause it to vibrate at the corresponding frequency (and thus produce the corresponding note).</t>
+    </r>
+  </si>
+  <si>
+    <t>X-Axis Steps per mm</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Feedrate Rounded</t>
+  </si>
+  <si>
+    <t>C6 Soprano C (High C)</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B♭5</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A♭5</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G♭5</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E♭5</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D♭5</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B♭4</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>E♭4</t>
+  </si>
+  <si>
+    <t>D♭4</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B♭3</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A♭3</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G♭3</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E♭3</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D♭3</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B♭2</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A♭2</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G♭2</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E♭2</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D♭2</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +425,58 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -284,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -292,6 +575,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -316,15 +608,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,720 +645,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>C6 Soprano C (High C)</v>
-          </cell>
-          <cell r="B8">
-            <v>1046.502</v>
-          </cell>
-          <cell r="C8">
-            <v>784.87649999999996</v>
-          </cell>
-          <cell r="D8">
-            <v>785</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>B5</v>
-          </cell>
-          <cell r="B9">
-            <v>987.76660000000004</v>
-          </cell>
-          <cell r="C9">
-            <v>740.82494999999994</v>
-          </cell>
-          <cell r="D9">
-            <v>741</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>B♭5</v>
-          </cell>
-          <cell r="B10">
-            <v>932.32749999999999</v>
-          </cell>
-          <cell r="C10">
-            <v>699.24562500000002</v>
-          </cell>
-          <cell r="D10">
-            <v>699</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>A5</v>
-          </cell>
-          <cell r="B11">
-            <v>880</v>
-          </cell>
-          <cell r="C11">
-            <v>660</v>
-          </cell>
-          <cell r="D11">
-            <v>660</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>A♭5</v>
-          </cell>
-          <cell r="B12">
-            <v>830.60940000000005</v>
-          </cell>
-          <cell r="C12">
-            <v>622.95705000000009</v>
-          </cell>
-          <cell r="D12">
-            <v>623</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>G5</v>
-          </cell>
-          <cell r="B13">
-            <v>783.99090000000001</v>
-          </cell>
-          <cell r="C13">
-            <v>587.99317499999995</v>
-          </cell>
-          <cell r="D13">
-            <v>588</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>G♭5</v>
-          </cell>
-          <cell r="B14">
-            <v>739.98879999999997</v>
-          </cell>
-          <cell r="C14">
-            <v>554.99160000000006</v>
-          </cell>
-          <cell r="D14">
-            <v>555</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>F5</v>
-          </cell>
-          <cell r="B15">
-            <v>698.45650000000001</v>
-          </cell>
-          <cell r="C15">
-            <v>523.84237499999995</v>
-          </cell>
-          <cell r="D15">
-            <v>524</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>E5</v>
-          </cell>
-          <cell r="B16">
-            <v>659.25509999999997</v>
-          </cell>
-          <cell r="C16">
-            <v>494.44132499999995</v>
-          </cell>
-          <cell r="D16">
-            <v>494</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>E♭5</v>
-          </cell>
-          <cell r="B17">
-            <v>622.25400000000002</v>
-          </cell>
-          <cell r="C17">
-            <v>466.69049999999999</v>
-          </cell>
-          <cell r="D17">
-            <v>467</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>D5</v>
-          </cell>
-          <cell r="B18">
-            <v>587.32950000000005</v>
-          </cell>
-          <cell r="C18">
-            <v>440.49712500000004</v>
-          </cell>
-          <cell r="D18">
-            <v>440</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>D♭5</v>
-          </cell>
-          <cell r="B19">
-            <v>554.36530000000005</v>
-          </cell>
-          <cell r="C19">
-            <v>415.77397500000006</v>
-          </cell>
-          <cell r="D19">
-            <v>416</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>C5</v>
-          </cell>
-          <cell r="B20">
-            <v>523.25109999999995</v>
-          </cell>
-          <cell r="C20">
-            <v>392.43832499999996</v>
-          </cell>
-          <cell r="D20">
-            <v>392</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>B4</v>
-          </cell>
-          <cell r="B21">
-            <v>493.88330000000002</v>
-          </cell>
-          <cell r="C21">
-            <v>370.41247499999997</v>
-          </cell>
-          <cell r="D21">
-            <v>370</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>B♭4</v>
-          </cell>
-          <cell r="B22">
-            <v>466.16379999999998</v>
-          </cell>
-          <cell r="C22">
-            <v>349.62284999999997</v>
-          </cell>
-          <cell r="D22">
-            <v>350</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>A4</v>
-          </cell>
-          <cell r="B23">
-            <v>440</v>
-          </cell>
-          <cell r="C23">
-            <v>330</v>
-          </cell>
-          <cell r="D23">
-            <v>330</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>A♭4</v>
-          </cell>
-          <cell r="B24">
-            <v>415.30470000000003</v>
-          </cell>
-          <cell r="C24">
-            <v>311.47852500000005</v>
-          </cell>
-          <cell r="D24">
-            <v>311</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>G4</v>
-          </cell>
-          <cell r="B25">
-            <v>391.99540000000002</v>
-          </cell>
-          <cell r="C25">
-            <v>293.99655000000001</v>
-          </cell>
-          <cell r="D25">
-            <v>294</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>G♭4</v>
-          </cell>
-          <cell r="B26">
-            <v>369.99439999999998</v>
-          </cell>
-          <cell r="C26">
-            <v>277.49580000000003</v>
-          </cell>
-          <cell r="D26">
-            <v>277</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>F4</v>
-          </cell>
-          <cell r="B27">
-            <v>349.22820000000002</v>
-          </cell>
-          <cell r="C27">
-            <v>261.92115000000001</v>
-          </cell>
-          <cell r="D27">
-            <v>262</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>E4</v>
-          </cell>
-          <cell r="B28">
-            <v>329.62759999999997</v>
-          </cell>
-          <cell r="C28">
-            <v>247.22069999999999</v>
-          </cell>
-          <cell r="D28">
-            <v>247</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>E♭4</v>
-          </cell>
-          <cell r="B29">
-            <v>311.12700000000001</v>
-          </cell>
-          <cell r="C29">
-            <v>233.34524999999999</v>
-          </cell>
-          <cell r="D29">
-            <v>233</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>D4</v>
-          </cell>
-          <cell r="B30">
-            <v>293.66480000000001</v>
-          </cell>
-          <cell r="C30">
-            <v>220.24859999999998</v>
-          </cell>
-          <cell r="D30">
-            <v>220</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>D♭4</v>
-          </cell>
-          <cell r="B31">
-            <v>277.18259999999998</v>
-          </cell>
-          <cell r="C31">
-            <v>207.88694999999998</v>
-          </cell>
-          <cell r="D31">
-            <v>208</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>C4</v>
-          </cell>
-          <cell r="B32">
-            <v>261.62560000000002</v>
-          </cell>
-          <cell r="C32">
-            <v>196.21920000000003</v>
-          </cell>
-          <cell r="D32">
-            <v>196</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>B3</v>
-          </cell>
-          <cell r="B33">
-            <v>246.9417</v>
-          </cell>
-          <cell r="C33">
-            <v>185.20627500000001</v>
-          </cell>
-          <cell r="D33">
-            <v>185</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>B♭3</v>
-          </cell>
-          <cell r="B34">
-            <v>233.08189999999999</v>
-          </cell>
-          <cell r="C34">
-            <v>174.81142499999999</v>
-          </cell>
-          <cell r="D34">
-            <v>175</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>A3</v>
-          </cell>
-          <cell r="B35">
-            <v>220</v>
-          </cell>
-          <cell r="C35">
-            <v>165</v>
-          </cell>
-          <cell r="D35">
-            <v>165</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>A♭3</v>
-          </cell>
-          <cell r="B36">
-            <v>207.6523</v>
-          </cell>
-          <cell r="C36">
-            <v>155.73922499999998</v>
-          </cell>
-          <cell r="D36">
-            <v>156</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>G3</v>
-          </cell>
-          <cell r="B37">
-            <v>195.99770000000001</v>
-          </cell>
-          <cell r="C37">
-            <v>146.99827500000001</v>
-          </cell>
-          <cell r="D37">
-            <v>147</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>G♭3</v>
-          </cell>
-          <cell r="B38">
-            <v>184.99719999999999</v>
-          </cell>
-          <cell r="C38">
-            <v>138.74790000000002</v>
-          </cell>
-          <cell r="D38">
-            <v>139</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39" t="str">
-            <v>F3</v>
-          </cell>
-          <cell r="B39">
-            <v>174.61410000000001</v>
-          </cell>
-          <cell r="C39">
-            <v>130.96057500000001</v>
-          </cell>
-          <cell r="D39">
-            <v>131</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40" t="str">
-            <v>E3</v>
-          </cell>
-          <cell r="B40">
-            <v>164.81379999999999</v>
-          </cell>
-          <cell r="C40">
-            <v>123.61035</v>
-          </cell>
-          <cell r="D40">
-            <v>124</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41" t="str">
-            <v>E♭3</v>
-          </cell>
-          <cell r="B41">
-            <v>155.5635</v>
-          </cell>
-          <cell r="C41">
-            <v>116.672625</v>
-          </cell>
-          <cell r="D41">
-            <v>117</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42" t="str">
-            <v>D3</v>
-          </cell>
-          <cell r="B42">
-            <v>146.83240000000001</v>
-          </cell>
-          <cell r="C42">
-            <v>110.12429999999999</v>
-          </cell>
-          <cell r="D42">
-            <v>110</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43" t="str">
-            <v>D♭3</v>
-          </cell>
-          <cell r="B43">
-            <v>138.59129999999999</v>
-          </cell>
-          <cell r="C43">
-            <v>103.94347499999999</v>
-          </cell>
-          <cell r="D43">
-            <v>104</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44" t="str">
-            <v>C3</v>
-          </cell>
-          <cell r="B44">
-            <v>130.81280000000001</v>
-          </cell>
-          <cell r="C44">
-            <v>98.109600000000015</v>
-          </cell>
-          <cell r="D44">
-            <v>98</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45" t="str">
-            <v>B2</v>
-          </cell>
-          <cell r="B45">
-            <v>123.4708</v>
-          </cell>
-          <cell r="C45">
-            <v>92.603099999999998</v>
-          </cell>
-          <cell r="D45">
-            <v>93</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46" t="str">
-            <v>B♭2</v>
-          </cell>
-          <cell r="B46">
-            <v>116.54089999999999</v>
-          </cell>
-          <cell r="C46">
-            <v>87.405675000000002</v>
-          </cell>
-          <cell r="D46">
-            <v>87</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47" t="str">
-            <v>A2</v>
-          </cell>
-          <cell r="B47">
-            <v>110</v>
-          </cell>
-          <cell r="C47">
-            <v>82.5</v>
-          </cell>
-          <cell r="D47">
-            <v>83</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48" t="str">
-            <v>A♭2</v>
-          </cell>
-          <cell r="B48">
-            <v>103.8262</v>
-          </cell>
-          <cell r="C48">
-            <v>77.869650000000007</v>
-          </cell>
-          <cell r="D48">
-            <v>78</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49" t="str">
-            <v>G2</v>
-          </cell>
-          <cell r="B49">
-            <v>97.998859999999993</v>
-          </cell>
-          <cell r="C49">
-            <v>73.499144999999999</v>
-          </cell>
-          <cell r="D49">
-            <v>73</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50" t="str">
-            <v>G♭2</v>
-          </cell>
-          <cell r="B50">
-            <v>92.498609999999999</v>
-          </cell>
-          <cell r="C50">
-            <v>69.373957499999989</v>
-          </cell>
-          <cell r="D50">
-            <v>69</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51" t="str">
-            <v>F2</v>
-          </cell>
-          <cell r="B51">
-            <v>87.307060000000007</v>
-          </cell>
-          <cell r="C51">
-            <v>65.480294999999998</v>
-          </cell>
-          <cell r="D51">
-            <v>65</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52" t="str">
-            <v>E2</v>
-          </cell>
-          <cell r="B52">
-            <v>82.406890000000004</v>
-          </cell>
-          <cell r="C52">
-            <v>61.805167500000003</v>
-          </cell>
-          <cell r="D52">
-            <v>62</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53" t="str">
-            <v>E♭2</v>
-          </cell>
-          <cell r="B53">
-            <v>77.781750000000002</v>
-          </cell>
-          <cell r="C53">
-            <v>58.336312499999998</v>
-          </cell>
-          <cell r="D53">
-            <v>58</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54" t="str">
-            <v>D2</v>
-          </cell>
-          <cell r="B54">
-            <v>73.41619</v>
-          </cell>
-          <cell r="C54">
-            <v>55.062142500000007</v>
-          </cell>
-          <cell r="D54">
-            <v>55</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55" t="str">
-            <v>D♭2</v>
-          </cell>
-          <cell r="B55">
-            <v>69.295659999999998</v>
-          </cell>
-          <cell r="C55">
-            <v>51.971744999999999</v>
-          </cell>
-          <cell r="D55">
-            <v>52</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56" t="str">
-            <v>C2</v>
-          </cell>
-          <cell r="B56">
-            <v>65.406390000000002</v>
-          </cell>
-          <cell r="C56">
-            <v>49.054792500000005</v>
-          </cell>
-          <cell r="D56">
-            <v>49</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58" t="str">
-            <v>R</v>
-          </cell>
-          <cell r="B58">
-            <v>20</v>
-          </cell>
-          <cell r="C58">
-            <v>15</v>
-          </cell>
-          <cell r="D58">
-            <v>15</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1338,12 +929,38 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C5" dT="2020-07-09T15:00:00.86" personId="{037F1714-9E98-4340-8A90-6342728E298A}" id="{6020CAEE-D306-4F1F-BB7F-A6CB184BC50D}">
+    <text>X-Axis maximum feedrate = 500 mm/min</text>
+  </threadedComment>
+  <threadedComment ref="C7" dT="2020-07-09T14:58:41.86" personId="{037F1714-9E98-4340-8A90-6342728E298A}" id="{2E6EC54C-154F-40FF-9749-75F374B15888}">
+    <text>Feedrate = (Frequency * 60) / Steps per mm</text>
+  </threadedComment>
+  <threadedComment ref="A20" dT="2020-07-09T16:05:51.87" personId="{037F1714-9E98-4340-8A90-6342728E298A}" id="{1528385D-5D7B-4677-AEC9-9C49986BDF3B}">
+    <text>Tenor C</text>
+  </threadedComment>
+  <threadedComment ref="A32" dT="2020-07-09T16:06:07.15" personId="{037F1714-9E98-4340-8A90-6342728E298A}" id="{9F3A1DCB-0146-47AA-B870-7E7AB149BD73}">
+    <text>Middle C</text>
+  </threadedComment>
+  <threadedComment ref="A56" dT="2020-07-09T16:06:16.63" personId="{037F1714-9E98-4340-8A90-6342728E298A}" id="{BE0622C6-345E-43CD-B3D2-D7804500A6B7}">
+    <text>Deep C</text>
+  </threadedComment>
+  <threadedComment ref="A58" dT="2020-07-09T19:14:23.84" personId="{037F1714-9E98-4340-8A90-6342728E298A}" id="{84CA6D1B-466B-4B66-BFE4-2488886A4766}">
+    <text>Rest</text>
+  </threadedComment>
+  <threadedComment ref="B58" dT="2020-07-09T19:20:58.60" personId="{037F1714-9E98-4340-8A90-6342728E298A}" id="{AA34F346-5608-41B5-BA45-AD2A51502823}">
+    <text>This frequency is too low for human hearing to detect.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,44 +974,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="F4" s="15" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="F4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16">
         <v>160</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="17"/>
       <c r="F5" s="4" t="str">
         <f>_xlfn.CONCAT("G17 \nM350 X1 \nG91 ","\n",E8,"\n",E9,"\n",E10,"\n",E11,"\n",E12,"\n",E13,"\n",E14,"\n",E15,"\n",E16,"\n",E17,"\n",E18,"\n",E19,"\n",E20,"\n",E21,"\n",E22,"\n",E23,"\n",E24,"\n",E25,"\n",E26,"\n",E27,"\n",E28,"\n",E29,"\n",E30,"\n",E31,"\n",E32,"\n",E33,"\n",E34,"\n",E35,"\n",E36,"\n",E37,"\n",E38,"\n",E39,"\n",E40,"\n",E41,"\n",E42,"\n",E43,"\n",E44,"\n",E45,"\n",E46,"\n",E47,"\n",E48,"\n",E49,"\n",E50,"\n",E51,"\n",E52,"\n",E53,"\n",E54,"\n",E55,"\n",E56,"\n",E57,"\n",E58,"\n",E59,"\n",E60,"\n",E61,"\n",E62,"\n",E63,"\n",E64,"\n",E65,"\n",E66,"\n",E67,"\n",E68,"\n",E69,"\n",E70,"\n",E71,"\n",E72,"\n",E73,"\n",E74,"\n",E75,"\n",E76,"\n",E77,"\n",E78,"\n",E79,"\n",E80,"\n",E81,"\n",E82,"\n",E83,"\n",E84,"\n",E85,"\n",E86,"\n",E87,"\n",E88,"\n",E89,"\n",E90)</f>
         <v>G17 \nM350 X1 \nG91 \nG0 X0.0234375 F15\nG0 X0.30625 F196\nG0 X0.409375 F262\nG0 X0.4859375 F311\nG0 X1.546875 F330\nG0 X0.30625 F196\nG0 X0.409375 F262\nG0 X0.4859375 F311\nG0 X1.03125 F330\nG0 X2.0625 F330\nG0 X0.0234375 F15\nG0 X0.34375 F220\nG0 X0.4328125 F277\nG0 X0.4859375 F311\nG0 X1.546875 F330\nG0 X0.34375 F220\nG0 X0.4328125 F277\nG0 X0.4859375 F311\nG0 X1.03125 F330\nG0 X2.0625 F330\nG0 X0.0234375 F15\nG0 X0.30625 F196\nG0 X0.3859375 F247\nG0 X0.4328125 F277\nG0 X1.4578125 F311\nG0 X0.30625 F196\nG0 X0.3859375 F247\nG0 X0.4328125 F277\nG0 X2.915625 F311\nG0 X0.0234375 F15\nG0 X0.4328125 F277\nG0 X0.4859375 F311\nG0 X0.4328125 F277\nG0 X1.73125 F277\nG0 X0.1875 F15\nG0 X0.0234375 F15\nG0 X0.515625 F330\nG0 X0.6125 F392\nG0 X0.515625 F330\nG0 X5.83125 F311\nG0 X0.046875 F15\nG0 X0.6125 F196\nG0 X0.30625 F196\nG0 X1.546875 F330\nG0 X1.4578125 F311\nG0 X0.4328125 F277\nG0 X0.865625 F277\nG0 X0.6125 F196\nG0 X1.54375 F247\nG0 X0.3859375 F247\nG0 X0.4328125 F277\nG0 X0.3859375 F247\nG0 X0.34375 F220\nG0 X2.75 F220\nG0 X0.046875 F15\nG0 X0.6125 F196\nG0 X0.30625 F196\nG0 X1.4578125 F311\nG0 X1.2984375 F277\nG0 X0.3859375 F247\nG0 X0.771875 F247\nG0 X0.6875 F220\nG0 X1.225 F196\nG0 X0.34375 F220\nG0 X0.3859375 F247\nG0 X0.34375 F220\nG0 X0.30625 F196\nG0 X2.45 F196\nG0 X0.046875 F15\nG0 X0.6125 F196\nG0 X0.30625 F196\nG0 X1.546875 F330\nG0 X1.4578125 F311\nG0 X0.4328125 F277\nG0 X0.865625 F277\nG0 X0.6125 F196\nG0 X1.54375 F247\nG0 X0.3859375 F247\nG0 X0.4328125 F277\nG0 X0.3859375 F247\nG0 X0.34375 F220\nG0 X1.03125 F220\nG0 X0.6125 F196</v>
@@ -1425,7 +1042,7 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <f>VLOOKUP(A8,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A8,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>15</v>
       </c>
       <c r="C8" s="2">
@@ -1445,7 +1062,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <f>VLOOKUP(A9,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A9,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C9" s="2">
@@ -1465,7 +1082,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <f>VLOOKUP(A10,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A10,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>262</v>
       </c>
       <c r="C10" s="2">
@@ -1486,7 +1103,7 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <f>VLOOKUP(A11,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A11,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C11" s="2">
@@ -1506,7 +1123,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <f>VLOOKUP(A12,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A12,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>330</v>
       </c>
       <c r="C12" s="2">
@@ -1526,7 +1143,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <f>VLOOKUP(A13,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A13,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C13" s="2">
@@ -1546,7 +1163,7 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <f>VLOOKUP(A14,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A14,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>262</v>
       </c>
       <c r="C14" s="2">
@@ -1566,7 +1183,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <f>VLOOKUP(A15,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A15,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C15" s="2">
@@ -1586,7 +1203,7 @@
         <v>12</v>
       </c>
       <c r="B16">
-        <f>VLOOKUP(A16,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A16,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>330</v>
       </c>
       <c r="C16" s="2">
@@ -1606,7 +1223,7 @@
         <v>12</v>
       </c>
       <c r="B17">
-        <f>VLOOKUP(A17,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A17,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>330</v>
       </c>
       <c r="C17" s="2">
@@ -1626,7 +1243,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <f>VLOOKUP(A18,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A18,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>15</v>
       </c>
       <c r="C18" s="2">
@@ -1646,7 +1263,7 @@
         <v>8</v>
       </c>
       <c r="B19">
-        <f>VLOOKUP(A19,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A19,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>220</v>
       </c>
       <c r="C19" s="2">
@@ -1666,7 +1283,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <f>VLOOKUP(A20,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A20,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C20" s="2">
@@ -1686,7 +1303,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <f>VLOOKUP(A21,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A21,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C21" s="2">
@@ -1706,7 +1323,7 @@
         <v>12</v>
       </c>
       <c r="B22">
-        <f>VLOOKUP(A22,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A22,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>330</v>
       </c>
       <c r="C22" s="2">
@@ -1726,7 +1343,7 @@
         <v>8</v>
       </c>
       <c r="B23">
-        <f>VLOOKUP(A23,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A23,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>220</v>
       </c>
       <c r="C23" s="2">
@@ -1746,7 +1363,7 @@
         <v>17</v>
       </c>
       <c r="B24">
-        <f>VLOOKUP(A24,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A24,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C24" s="2">
@@ -1766,7 +1383,7 @@
         <v>18</v>
       </c>
       <c r="B25">
-        <f>VLOOKUP(A25,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A25,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C25" s="2">
@@ -1786,7 +1403,7 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <f>VLOOKUP(A26,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A26,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>330</v>
       </c>
       <c r="C26" s="2">
@@ -1806,7 +1423,7 @@
         <v>12</v>
       </c>
       <c r="B27">
-        <f>VLOOKUP(A27,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A27,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>330</v>
       </c>
       <c r="C27" s="2">
@@ -1826,7 +1443,7 @@
         <v>16</v>
       </c>
       <c r="B28">
-        <f>VLOOKUP(A28,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A28,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>15</v>
       </c>
       <c r="C28" s="2">
@@ -1846,7 +1463,7 @@
         <v>15</v>
       </c>
       <c r="B29">
-        <f>VLOOKUP(A29,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A29,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C29" s="2">
@@ -1867,7 +1484,7 @@
         <v>13</v>
       </c>
       <c r="B30">
-        <f>VLOOKUP(A30,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A30,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C30" s="2">
@@ -1887,7 +1504,7 @@
         <v>17</v>
       </c>
       <c r="B31">
-        <f>VLOOKUP(A31,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A31,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C31" s="2">
@@ -1907,7 +1524,7 @@
         <v>18</v>
       </c>
       <c r="B32">
-        <f>VLOOKUP(A32,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A32,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C32" s="2">
@@ -1927,7 +1544,7 @@
         <v>15</v>
       </c>
       <c r="B33">
-        <f>VLOOKUP(A33,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A33,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C33" s="2">
@@ -1947,7 +1564,7 @@
         <v>13</v>
       </c>
       <c r="B34">
-        <f>VLOOKUP(A34,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A34,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C34" s="2">
@@ -1967,7 +1584,7 @@
         <v>17</v>
       </c>
       <c r="B35">
-        <f>VLOOKUP(A35,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A35,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C35" s="2">
@@ -1987,7 +1604,7 @@
         <v>18</v>
       </c>
       <c r="B36">
-        <f>VLOOKUP(A36,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A36,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C36" s="2">
@@ -2007,7 +1624,7 @@
         <v>16</v>
       </c>
       <c r="B37">
-        <f>VLOOKUP(A37,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A37,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>15</v>
       </c>
       <c r="C37" s="2">
@@ -2027,7 +1644,7 @@
         <v>17</v>
       </c>
       <c r="B38">
-        <f>VLOOKUP(A38,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A38,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C38" s="2">
@@ -2047,7 +1664,7 @@
         <v>18</v>
       </c>
       <c r="B39">
-        <f>VLOOKUP(A39,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A39,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C39" s="2">
@@ -2067,7 +1684,7 @@
         <v>17</v>
       </c>
       <c r="B40">
-        <f>VLOOKUP(A40,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A40,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C40" s="2">
@@ -2087,7 +1704,7 @@
         <v>17</v>
       </c>
       <c r="B41">
-        <f>VLOOKUP(A41,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A41,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C41" s="2">
@@ -2107,7 +1724,7 @@
         <v>16</v>
       </c>
       <c r="B42">
-        <f>VLOOKUP(A42,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A42,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>15</v>
       </c>
       <c r="C42" s="2">
@@ -2127,7 +1744,7 @@
         <v>16</v>
       </c>
       <c r="B43">
-        <f>VLOOKUP(A43,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A43,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>15</v>
       </c>
       <c r="C43" s="2">
@@ -2147,7 +1764,7 @@
         <v>12</v>
       </c>
       <c r="B44">
-        <f>VLOOKUP(A44,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A44,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>330</v>
       </c>
       <c r="C44" s="2">
@@ -2167,7 +1784,7 @@
         <v>11</v>
       </c>
       <c r="B45">
-        <f>VLOOKUP(A45,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A45,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>392</v>
       </c>
       <c r="C45" s="2">
@@ -2187,7 +1804,7 @@
         <v>12</v>
       </c>
       <c r="B46">
-        <f>VLOOKUP(A46,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A46,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>330</v>
       </c>
       <c r="C46" s="2">
@@ -2207,7 +1824,7 @@
         <v>18</v>
       </c>
       <c r="B47">
-        <f>VLOOKUP(A47,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A47,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C47" s="2">
@@ -2227,7 +1844,7 @@
         <v>16</v>
       </c>
       <c r="B48">
-        <f>VLOOKUP(A48,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A48,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>15</v>
       </c>
       <c r="C48" s="2">
@@ -2247,7 +1864,7 @@
         <v>15</v>
       </c>
       <c r="B49">
-        <f>VLOOKUP(A49,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A49,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C49" s="2">
@@ -2267,7 +1884,7 @@
         <v>15</v>
       </c>
       <c r="B50">
-        <f>VLOOKUP(A50,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A50,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C50" s="2">
@@ -2287,7 +1904,7 @@
         <v>12</v>
       </c>
       <c r="B51">
-        <f>VLOOKUP(A51,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A51,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>330</v>
       </c>
       <c r="C51" s="2">
@@ -2307,7 +1924,7 @@
         <v>18</v>
       </c>
       <c r="B52">
-        <f>VLOOKUP(A52,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A52,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C52" s="2">
@@ -2327,7 +1944,7 @@
         <v>17</v>
       </c>
       <c r="B53">
-        <f>VLOOKUP(A53,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A53,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C53" s="2">
@@ -2347,7 +1964,7 @@
         <v>17</v>
       </c>
       <c r="B54">
-        <f>VLOOKUP(A54,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A54,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C54" s="2">
@@ -2367,7 +1984,7 @@
         <v>15</v>
       </c>
       <c r="B55">
-        <f>VLOOKUP(A55,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A55,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C55" s="2">
@@ -2387,7 +2004,7 @@
         <v>13</v>
       </c>
       <c r="B56">
-        <f>VLOOKUP(A56,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A56,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C56" s="2">
@@ -2407,7 +2024,7 @@
         <v>13</v>
       </c>
       <c r="B57">
-        <f>VLOOKUP(A57,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A57,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C57" s="2">
@@ -2427,7 +2044,7 @@
         <v>17</v>
       </c>
       <c r="B58">
-        <f>VLOOKUP(A58,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A58,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C58" s="2">
@@ -2447,7 +2064,7 @@
         <v>13</v>
       </c>
       <c r="B59">
-        <f>VLOOKUP(A59,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A59,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C59" s="2">
@@ -2467,7 +2084,7 @@
         <v>8</v>
       </c>
       <c r="B60">
-        <f>VLOOKUP(A60,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A60,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>220</v>
       </c>
       <c r="C60" s="2">
@@ -2487,7 +2104,7 @@
         <v>8</v>
       </c>
       <c r="B61">
-        <f>VLOOKUP(A61,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A61,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>220</v>
       </c>
       <c r="C61" s="2">
@@ -2507,7 +2124,7 @@
         <v>16</v>
       </c>
       <c r="B62">
-        <f>VLOOKUP(A62,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A62,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>15</v>
       </c>
       <c r="C62" s="2">
@@ -2527,7 +2144,7 @@
         <v>15</v>
       </c>
       <c r="B63">
-        <f>VLOOKUP(A63,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A63,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C63" s="2">
@@ -2547,7 +2164,7 @@
         <v>15</v>
       </c>
       <c r="B64">
-        <f>VLOOKUP(A64,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A64,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C64" s="2">
@@ -2567,7 +2184,7 @@
         <v>18</v>
       </c>
       <c r="B65">
-        <f>VLOOKUP(A65,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A65,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C65" s="2">
@@ -2587,7 +2204,7 @@
         <v>17</v>
       </c>
       <c r="B66">
-        <f>VLOOKUP(A66,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A66,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C66" s="2">
@@ -2607,7 +2224,7 @@
         <v>13</v>
       </c>
       <c r="B67">
-        <f>VLOOKUP(A67,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A67,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C67" s="2">
@@ -2627,7 +2244,7 @@
         <v>13</v>
       </c>
       <c r="B68">
-        <f>VLOOKUP(A68,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A68,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C68" s="2">
@@ -2647,7 +2264,7 @@
         <v>8</v>
       </c>
       <c r="B69">
-        <f>VLOOKUP(A69,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A69,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>220</v>
       </c>
       <c r="C69" s="2">
@@ -2667,7 +2284,7 @@
         <v>15</v>
       </c>
       <c r="B70">
-        <f>VLOOKUP(A70,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A70,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C70" s="2">
@@ -2687,7 +2304,7 @@
         <v>8</v>
       </c>
       <c r="B71">
-        <f>VLOOKUP(A71,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A71,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>220</v>
       </c>
       <c r="C71" s="2">
@@ -2707,7 +2324,7 @@
         <v>13</v>
       </c>
       <c r="B72">
-        <f>VLOOKUP(A72,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A72,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C72" s="2">
@@ -2727,7 +2344,7 @@
         <v>8</v>
       </c>
       <c r="B73">
-        <f>VLOOKUP(A73,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A73,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>220</v>
       </c>
       <c r="C73" s="2">
@@ -2747,7 +2364,7 @@
         <v>15</v>
       </c>
       <c r="B74">
-        <f>VLOOKUP(A74,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A74,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C74" s="2">
@@ -2767,7 +2384,7 @@
         <v>15</v>
       </c>
       <c r="B75">
-        <f>VLOOKUP(A75,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A75,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C75" s="2">
@@ -2787,7 +2404,7 @@
         <v>16</v>
       </c>
       <c r="B76">
-        <f>VLOOKUP(A76,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A76,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>15</v>
       </c>
       <c r="C76" s="2">
@@ -2807,7 +2424,7 @@
         <v>15</v>
       </c>
       <c r="B77">
-        <f>VLOOKUP(A77,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A77,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C77" s="2">
@@ -2827,7 +2444,7 @@
         <v>15</v>
       </c>
       <c r="B78">
-        <f>VLOOKUP(A78,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A78,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C78" s="2">
@@ -2847,7 +2464,7 @@
         <v>12</v>
       </c>
       <c r="B79">
-        <f>VLOOKUP(A79,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A79,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>330</v>
       </c>
       <c r="C79" s="2">
@@ -2867,7 +2484,7 @@
         <v>18</v>
       </c>
       <c r="B80">
-        <f>VLOOKUP(A80,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A80,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>311</v>
       </c>
       <c r="C80" s="2">
@@ -2887,7 +2504,7 @@
         <v>17</v>
       </c>
       <c r="B81">
-        <f>VLOOKUP(A81,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A81,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C81" s="2">
@@ -2907,7 +2524,7 @@
         <v>17</v>
       </c>
       <c r="B82">
-        <f>VLOOKUP(A82,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A82,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C82" s="2">
@@ -2927,7 +2544,7 @@
         <v>15</v>
       </c>
       <c r="B83">
-        <f>VLOOKUP(A83,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A83,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C83" s="2">
@@ -2947,7 +2564,7 @@
         <v>13</v>
       </c>
       <c r="B84">
-        <f>VLOOKUP(A84,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A84,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C84" s="2">
@@ -2967,7 +2584,7 @@
         <v>13</v>
       </c>
       <c r="B85">
-        <f>VLOOKUP(A85,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A85,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C85" s="2">
@@ -2987,7 +2604,7 @@
         <v>17</v>
       </c>
       <c r="B86">
-        <f>VLOOKUP(A86,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A86,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>277</v>
       </c>
       <c r="C86" s="2">
@@ -3007,7 +2624,7 @@
         <v>13</v>
       </c>
       <c r="B87">
-        <f>VLOOKUP(A87,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A87,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>247</v>
       </c>
       <c r="C87" s="2">
@@ -3027,7 +2644,7 @@
         <v>8</v>
       </c>
       <c r="B88">
-        <f>VLOOKUP(A88,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A88,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>220</v>
       </c>
       <c r="C88" s="2">
@@ -3047,7 +2664,7 @@
         <v>8</v>
       </c>
       <c r="B89">
-        <f>VLOOKUP(A89,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A89,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>220</v>
       </c>
       <c r="C89" s="2">
@@ -3067,7 +2684,7 @@
         <v>15</v>
       </c>
       <c r="B90">
-        <f>VLOOKUP(A90,[1]Sheet1!$A$8:$D$58,4,FALSE)</f>
+        <f>VLOOKUP(A90,'Notes to Feedrate'!$A$8:$D$58,4,FALSE)</f>
         <v>196</v>
       </c>
       <c r="C90" s="2">
@@ -3095,4 +2712,881 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0313B5E-A5DF-4BF5-93EB-5CA34AAFDD01}">
+  <dimension ref="A1:D58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21">
+        <v>80</v>
+      </c>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="24">
+        <v>1046.502</v>
+      </c>
+      <c r="C8" s="23">
+        <f>(B8*60)/$C$5</f>
+        <v>784.87649999999996</v>
+      </c>
+      <c r="D8" s="23">
+        <f>ROUND(C8,0)</f>
+        <v>785</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="24">
+        <v>987.76660000000004</v>
+      </c>
+      <c r="C9" s="23">
+        <f t="shared" ref="C9:C58" si="0">(B9*60)/$C$5</f>
+        <v>740.82494999999994</v>
+      </c>
+      <c r="D9" s="23">
+        <f t="shared" ref="D9:D58" si="1">ROUND(C9,0)</f>
+        <v>741</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="24">
+        <v>932.32749999999999</v>
+      </c>
+      <c r="C10" s="23">
+        <f t="shared" si="0"/>
+        <v>699.24562500000002</v>
+      </c>
+      <c r="D10" s="23">
+        <f t="shared" si="1"/>
+        <v>699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="25">
+        <v>880</v>
+      </c>
+      <c r="C11" s="23">
+        <f t="shared" si="0"/>
+        <v>660</v>
+      </c>
+      <c r="D11" s="23">
+        <f t="shared" si="1"/>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="24">
+        <v>830.60940000000005</v>
+      </c>
+      <c r="C12" s="23">
+        <f t="shared" si="0"/>
+        <v>622.95705000000009</v>
+      </c>
+      <c r="D12" s="23">
+        <f t="shared" si="1"/>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="24">
+        <v>783.99090000000001</v>
+      </c>
+      <c r="C13" s="23">
+        <f t="shared" si="0"/>
+        <v>587.99317499999995</v>
+      </c>
+      <c r="D13" s="23">
+        <f t="shared" si="1"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="24">
+        <v>739.98879999999997</v>
+      </c>
+      <c r="C14" s="23">
+        <f t="shared" si="0"/>
+        <v>554.99160000000006</v>
+      </c>
+      <c r="D14" s="23">
+        <f t="shared" si="1"/>
+        <v>555</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="24">
+        <v>698.45650000000001</v>
+      </c>
+      <c r="C15" s="23">
+        <f t="shared" si="0"/>
+        <v>523.84237499999995</v>
+      </c>
+      <c r="D15" s="23">
+        <f t="shared" si="1"/>
+        <v>524</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="24">
+        <v>659.25509999999997</v>
+      </c>
+      <c r="C16" s="23">
+        <f t="shared" si="0"/>
+        <v>494.44132499999995</v>
+      </c>
+      <c r="D16" s="23">
+        <f t="shared" si="1"/>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="26">
+        <v>622.25400000000002</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>466.69049999999999</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>467</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="26">
+        <v>587.32950000000005</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>440.49712500000004</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="26">
+        <v>554.36530000000005</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>415.77397500000006</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="26">
+        <v>523.25109999999995</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>392.43832499999996</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="26">
+        <v>493.88330000000002</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>370.41247499999997</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="26">
+        <v>466.16379999999998</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>349.62284999999997</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="27">
+        <v>440</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="26">
+        <v>415.30470000000003</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>311.47852500000005</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="26">
+        <v>391.99540000000002</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>293.99655000000001</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="26">
+        <v>369.99439999999998</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>277.49580000000003</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="26">
+        <v>349.22820000000002</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>261.92115000000001</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="26">
+        <v>329.62759999999997</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>247.22069999999999</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="26">
+        <v>311.12700000000001</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>233.34524999999999</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="26">
+        <v>293.66480000000001</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>220.24859999999998</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="26">
+        <v>277.18259999999998</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>207.88694999999998</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="28">
+        <v>261.62560000000002</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>196.21920000000003</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="26">
+        <v>246.9417</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>185.20627500000001</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="26">
+        <v>233.08189999999999</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>174.81142499999999</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="29">
+        <v>220</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="26">
+        <v>207.6523</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>155.73922499999998</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="26">
+        <v>195.99770000000001</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>146.99827500000001</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="26">
+        <v>184.99719999999999</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>138.74790000000002</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="26">
+        <v>174.61410000000001</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>130.96057500000001</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="26">
+        <v>164.81379999999999</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>123.61035</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="26">
+        <v>155.5635</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>116.672625</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="26">
+        <v>146.83240000000001</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>110.12429999999999</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="26">
+        <v>138.59129999999999</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>103.94347499999999</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="26">
+        <v>130.81280000000001</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>98.109600000000015</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="26">
+        <v>123.4708</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>92.603099999999998</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="26">
+        <v>116.54089999999999</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>87.405675000000002</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="29">
+        <v>110</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>82.5</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="26">
+        <v>103.8262</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>77.869650000000007</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="26">
+        <v>97.998859999999993</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>73.499144999999999</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="26">
+        <v>92.498609999999999</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>69.373957499999989</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="26">
+        <v>87.307060000000007</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>65.480294999999998</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="26">
+        <v>82.406890000000004</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>61.805167500000003</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="26">
+        <v>77.781750000000002</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>58.336312499999998</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="26">
+        <v>73.41619</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>55.062142500000007</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="26">
+        <v>69.295659999999998</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>51.971744999999999</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="26">
+        <v>65.406390000000002</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>49.054792500000005</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="26">
+        <v>20</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>